<commit_message>
fix: various task transformer improvements
for xlsx
- remove support for column "Version"
- add support for columns "goal_version", "rule_name_id", "rule_version"
- add support for profile-type generation "by-goal", "by-rule",
"by-control", "by-check"
- skip rows where control_id or goal_id is missing with complaint
- skip rows where control_id and goal_id are missing, after 100
consecutive terminate processing
- improve sotring of controls

for ocp4
- give warning (not failure) when unable to extract title from
compliance-as-code rule.yml
</commit_message>
<xml_diff>
--- a/tests/data/spread-sheet/bad_parameter_name_and_description.xlsx
+++ b/tests/data/spread-sheet/bad_parameter_name_and_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">ControlId</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">goal_name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rule_name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rule_version</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter
@@ -305,17 +314,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE3" activeCellId="0" sqref="AE3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AR2" activeCellId="0" sqref="AR2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
@@ -325,8 +334,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,11 +366,20 @@
       <c r="AN1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AP1" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,38 +387,43 @@
         <v>3000109</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AB2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AG2" s="12"/>
       <c r="AM2" s="13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AN2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ2" s="11"/>
+      <c r="AT2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU2" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: various task transformer improvements (#1100)
* fix: various task transformer improvements

for xlsx
- remove support for column "Version"
- add support for columns "goal_version", "rule_name_id", "rule_version"
- add support for profile-type generation "by-goal", "by-rule",
"by-control", "by-check"
- skip rows where control_id or goal_id is missing with complaint
- skip rows where control_id and goal_id are missing, after 100
consecutive terminate processing
- improve sotring of controls

for ocp4
- give warning (not failure) when unable to extract title from
compliance-as-code rule.yml

* "oscal-version": "1.0.2"

* Fix code smell.

* Do not emit parameters in the case of "by-control".

Co-authored-by: Frank Suits <47203786+fsuits@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/data/spread-sheet/bad_parameter_name_and_description.xlsx
+++ b/tests/data/spread-sheet/bad_parameter_name_and_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">ControlId</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">goal_name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rule_name_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rule_version</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter
@@ -305,17 +314,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE3" activeCellId="0" sqref="AE3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AR2" activeCellId="0" sqref="AR2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
@@ -325,8 +334,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,11 +366,20 @@
       <c r="AN1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AP1" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,38 +387,43 @@
         <v>3000109</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AB2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AG2" s="12"/>
       <c r="AM2" s="13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AN2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ2" s="11"/>
+      <c r="AT2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU2" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>